<commit_message>
Se exporta la programación general en Excel
</commit_message>
<xml_diff>
--- a/datos_intermedios/Data_Filtrada_Externos.xlsx
+++ b/datos_intermedios/Data_Filtrada_Externos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,55 +436,60 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Código de pedido</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Código de estación</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Nombre de estación</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Dirección</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Distrito</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Población</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Zona</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Cantidad de entrega</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Producto</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Descripción</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Código de centro de carga</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Nombre de centro de carga</t>
         </is>
@@ -493,53 +498,58 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>879436</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>1012160</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>EMP. DE TRANSPORTES TURISTICO OLANO</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Jirón Manuel Cisneros 492, La Victoria 15033</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>LA VICTORIA</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
         <v>8000</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>40002022</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>MAX-P PLUS DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>P600</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>TERMINAL CALLAO</t>
         </is>
@@ -548,53 +558,58 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>887593</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>1000156</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>PRODUCTOS DE ACERO CASSADO PRODAC S.A.C.</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Av. Nestor Gambetta 6429, Callao 07046</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>CALLAO</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
         <v>1000</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>40002014</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>MAX-P DIESEL B5 S50</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -603,53 +618,58 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>889587</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>1010840</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>GRIFO TRAPICHE S.R.L.</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Au. Chillón Trapiche 665, Comas 15316</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>COMAS</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
         <v>1000</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -658,53 +678,58 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>889583</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>1010840</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>GRIFO TRAPICHE S.R.L.</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Au. Chillón Trapiche 665, Comas 15316</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>COMAS</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
         <v>5000</v>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>40002019</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -713,53 +738,58 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>889580</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>1002721</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>INVERSIONES UCHIYAMA S.A.C.</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Av. La Mar 2382, San Miguel 15088</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>SAN MIGUEL</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
         <v>500</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>40002055</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -768,53 +798,58 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>889575</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>1002721</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>INVERSIONES UCHIYAMA S.A.C.</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Av. La Mar 2382, San Miguel 15088</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>SAN MIGUEL</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
         <v>1000</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
+      <c r="K7" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -823,53 +858,58 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>889562</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>1003274</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>ESTACION DE SERVICIOS LA MARINA S.A.C.</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Av. la Marina 405, La Perla 07011</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>LA PERLA</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
         <v>500</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>40002041</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>EXELON GASOHOL 90</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
+      <c r="K8" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -878,53 +918,58 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>889531</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>1003274</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>ESTACION DE SERVICIOS LA MARINA S.A.C.</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Av. la Marina 405, La Perla 07011</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>LA PERLA</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
         <v>1000</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>40002049</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>EXELON NITRO GASOHOL 95</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -933,53 +978,58 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>889531</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>1003274</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>ESTACION DE SERVICIOS LA MARINA S.A.C.</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Av. la Marina 405, La Perla 07011</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>LA PERLA</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
         <v>2000</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>40002057</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>EXELON NITRO GASOHOL 97</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
+      <c r="K10" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -988,53 +1038,58 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>889364</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>1011710</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>GASCORVILL S.A.C.</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Av. Pacasmayo 3, Callao 07031</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>CALLAO</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
         <v>500</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
+      <c r="K11" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1043,53 +1098,58 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>889363</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>1011710</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>GASCORVILL S.A.C.</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Av. Pacasmayo 3, Callao 07031</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>CALLAO</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
         <v>500</v>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>40002039</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
+      <c r="K12" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1098,53 +1158,58 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>889334</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>1015412</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>NEPTUNIA S.A.</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Av. Argentina 2085, Callao 07001</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>CALLAO</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
         <v>1500</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>40002017</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>PLUS DIESEL B5 S50</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
+      <c r="K13" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1153,53 +1218,58 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>889217</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>1002643</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>ESTACION CORMAR S.A.</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>W2XV+88P, Ate 15012</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>ATE</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G14" t="n">
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
         <v>6000</v>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>40002023</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>ENDURA DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1208,53 +1278,58 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>889215</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>1002607</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>AUTO SERVICIO LA PERLA S.A.</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Av. República de Venezuela, Bellavista 07011</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>LA PERLA</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
         <v>1500</v>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>40002041</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>EXELON GASOHOL 90</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="K15" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="L15" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1263,53 +1338,58 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>889215</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>1002607</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>AUTO SERVICIO LA PERLA S.A.</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Av. República de Venezuela, Bellavista 07011</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>LA PERLA</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
         <v>1000</v>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>40002049</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>EXELON NITRO GASOHOL 95</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
+      <c r="K16" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1318,53 +1398,58 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>889212</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>1002607</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>AUTO SERVICIO LA PERLA S.A.</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Av. República de Venezuela, Bellavista 07011</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>LA PERLA</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
         <v>1000</v>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>40002049</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>EXELON NITRO GASOHOL 95</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
+      <c r="K17" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1373,53 +1458,58 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>889199</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>1002607</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>AUTO SERVICIO LA PERLA S.A.</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Av. República de Venezuela, Bellavista 07011</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>LA PERLA</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
         <v>500</v>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>40002023</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>ENDURA DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
+      <c r="K18" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr">
+      <c r="L18" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1428,53 +1518,58 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>889157</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>1007571</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>SERVICIOS Y REPRESENTACIONES TACNA</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Av Bausate y Meza 1050, La Victoria 15018</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>LA VICTORIA</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F19" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
         <v>2000</v>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>40002049</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>EXELON NITRO GASOHOL 95</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
+      <c r="K19" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr">
+      <c r="L19" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1483,53 +1578,58 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>889150</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>1007571</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>SERVICIOS Y REPRESENTACIONES TACNA</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Av Bausate y Meza 1050, La Victoria 15018</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>LA VICTORIA</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F20" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G20" t="n">
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
         <v>1000</v>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>40002041</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>EXELON GASOHOL 90</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
+      <c r="K20" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr">
+      <c r="L20" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1538,53 +1638,58 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>889145</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>1007571</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>SERVICIOS Y REPRESENTACIONES TACNA</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Av Bausate y Meza 1050, La Victoria 15018</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>LA VICTORIA</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F21" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G21" t="n">
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
         <v>4000</v>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>40002023</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>ENDURA DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
+      <c r="K21" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1593,53 +1698,58 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>888957</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>1015412</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>NEPTUNIA S.A.</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Av. Argentina 2085, Callao 07001</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>CALLAO</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>PROV. CONST. DEL CALLAO</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
         <v>2500</v>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>40002017</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>PLUS DIESEL B5 S50</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
+      <c r="K22" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1648,53 +1758,58 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>888818</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>1013034</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>MOVIL BUS S.A.C.</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Av. Materiales 2215, Cercado de Lima 15081</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>CERCADO DE LIMA</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G23" t="n">
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
         <v>6000</v>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>40002014</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>MAX-P DIESEL B5 S50</t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
+      <c r="K23" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="L23" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1703,53 +1818,58 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>888704</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>1002634</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>INVERSIONES LUMARCO S.A.</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Carretera Central km 11.50 AAHH La Estrella, ATE, Lima</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>ATE</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F24" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G24" t="n">
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
         <v>1000</v>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>40002041</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>EXELON GASOHOL 90</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="L24" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1758,53 +1878,58 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>888704</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>1002634</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>INVERSIONES LUMARCO S.A.</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Carretera Central km 11.50 AAHH La Estrella, ATE, Lima</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>ATE</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F25" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G25" t="n">
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
         <v>1000</v>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>40002049</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>EXELON NITRO GASOHOL 95</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
+      <c r="K25" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="L25" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1813,53 +1938,58 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>888704</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>1002634</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>INVERSIONES LUMARCO S.A.</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Carretera Central km 11.50 AAHH La Estrella, ATE, Lima</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>ATE</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F26" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G26" t="n">
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
         <v>500</v>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>40002057</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>EXELON NITRO GASOHOL 97</t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
+      <c r="K26" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1868,53 +1998,58 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>888700</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>1002634</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>INVERSIONES LUMARCO S.A.</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Carretera Central km 11.50 AAHH La Estrella, ATE, Lima</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>ATE</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F27" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G27" t="n">
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
         <v>5000</v>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>40002023</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>ENDURA DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
+      <c r="K27" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="L27" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1923,53 +2058,58 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>888645</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>1011014</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>PACHACUTEC INVERSIONES GENERALES S.A.C.</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Av El Sol 127, Villa EL Salvador 15816</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>VILLA EL SALVADOR</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F28" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G28" t="n">
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
         <v>3500</v>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>40002019</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
+      <c r="K28" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="L28" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -1978,53 +2118,58 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>888641</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>1011014</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>PACHACUTEC INVERSIONES GENERALES S.A.C.</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Av El Sol 127, Villa EL Salvador 15816</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>VILLA EL SALVADOR</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F29" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G29" t="n">
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
         <v>1500</v>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>40002039</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2033,53 +2178,58 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>888641</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>1011014</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>PACHACUTEC INVERSIONES GENERALES S.A.C.</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>Av El Sol 127, Villa EL Salvador 15816</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>VILLA EL SALVADOR</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F30" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G30" t="n">
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
         <v>2000</v>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
+      <c r="K30" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="L30" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2088,53 +2238,58 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>888626</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>1002737</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>ESTACION DE SERVICIO NIAGARA S.R.L.</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>Jiron Elvira Garcia y Garcia 2790, Cercado de Lima 15081</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>CERCADO DE LIMA</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F31" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G31" t="n">
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
         <v>2000</v>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="I31" t="inlineStr">
         <is>
           <t>40002041</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
+      <c r="J31" t="inlineStr">
         <is>
           <t>EXELON GASOHOL 90</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
+      <c r="K31" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr">
+      <c r="L31" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2143,53 +2298,58 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>888626</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>1002737</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>ESTACION DE SERVICIO NIAGARA S.R.L.</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Jiron Elvira Garcia y Garcia 2790, Cercado de Lima 15081</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>CERCADO DE LIMA</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F32" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G32" t="n">
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
         <v>2000</v>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>40002049</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>EXELON NITRO GASOHOL 95</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
+      <c r="K32" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2198,53 +2358,58 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>888531</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>1010770</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>CORPORACION BLUE GAS S.A.C.</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Jirón el Alamo 121, Lima 15023</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>SANTIAGO DE SURCO</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F33" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G33" t="n">
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
         <v>1000</v>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="J33" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
+      <c r="K33" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr">
+      <c r="L33" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2253,53 +2418,58 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>888525</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>1010770</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>CORPORACION BLUE GAS S.A.C.</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>Jirón el Alamo 121, Lima 15023</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>SANTIAGO DE SURCO</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F34" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G34" t="n">
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
         <v>2000</v>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>40002039</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
+      <c r="K34" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr">
+      <c r="L34" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2308,53 +2478,58 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>888525</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>1010770</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>CORPORACION BLUE GAS S.A.C.</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Jirón el Alamo 121, Lima 15023</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>SANTIAGO DE SURCO</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F35" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G35" t="n">
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
         <v>4000</v>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="J35" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="K35" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="L35" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2363,53 +2538,58 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
+          <t>888525</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
           <t>1010770</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>CORPORACION BLUE GAS S.A.C.</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>Jirón el Alamo 121, Lima 15023</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>SANTIAGO DE SURCO</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F36" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G36" t="n">
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
         <v>2000</v>
       </c>
-      <c r="H36" t="inlineStr">
+      <c r="I36" t="inlineStr">
         <is>
           <t>40002055</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
+      <c r="J36" t="inlineStr">
         <is>
           <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
+      <c r="K36" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr">
+      <c r="L36" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2418,53 +2598,58 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>888425</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
           <t>1002706</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>GRIFOS TERESA DE CALCUTA S.A.</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Dsv.Manchay, Car. Cieneguilla Nro. S/n (Km 11.5, Pachacamac</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>PACHACAMAC</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F37" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G37" t="n">
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
         <v>500</v>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t>40002038</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
+      <c r="J37" t="inlineStr">
         <is>
           <t>GASOHOL 90</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
+      <c r="K37" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr">
+      <c r="L37" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2473,53 +2658,58 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
+          <t>888424</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
           <t>1002706</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>GRIFOS TERESA DE CALCUTA S.A.</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Dsv.Manchay, Car. Cieneguilla Nro. S/n (Km 11.5, Pachacamac</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>PACHACAMAC</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F38" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G38" t="n">
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
         <v>500</v>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t>40002025</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
+      <c r="J38" t="inlineStr">
         <is>
           <t>PLUS DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr">
+      <c r="K38" t="inlineStr">
         <is>
           <t>P611</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr">
+      <c r="L38" t="inlineStr">
         <is>
           <t>TERMINAL REFINERÍA PAMPILLA</t>
         </is>
@@ -2528,53 +2718,58 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
+          <t>889457</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
           <t>1003089</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>SERVICENTRO TACALA S.R.L.</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>Av San Martín, Chorrillos 15057</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>CHORRILLOS</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F39" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G39" t="n">
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
         <v>500</v>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>40002019</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr">
+      <c r="J39" t="inlineStr">
         <is>
           <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
+      <c r="K39" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr">
+      <c r="L39" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -2583,53 +2778,58 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>889452</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>1003089</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>SERVICENTRO TACALA S.R.L.</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>Av San Martín, Chorrillos 15057</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>CHORRILLOS</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F40" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G40" t="n">
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
         <v>1000</v>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="inlineStr">
         <is>
           <t>40002039</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="J40" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
+      <c r="K40" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr">
+      <c r="L40" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -2638,53 +2838,58 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>889452</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>1003089</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>SERVICENTRO TACALA S.R.L.</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Av San Martín, Chorrillos 15057</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>CHORRILLOS</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F41" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G41" t="n">
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
         <v>500</v>
       </c>
-      <c r="H41" t="inlineStr">
+      <c r="I41" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr">
+      <c r="J41" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
+      <c r="K41" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr">
+      <c r="L41" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -2693,53 +2898,58 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
+          <t>888644</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
           <t>1002685</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>ORGANIZACION FUTURO S.A.C.</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>Av. Javier Prado Este 6651, La Molina 15012</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>LA MOLINA</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F42" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G42" t="n">
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
         <v>500</v>
       </c>
-      <c r="H42" t="inlineStr">
+      <c r="I42" t="inlineStr">
         <is>
           <t>40002041</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
+      <c r="J42" t="inlineStr">
         <is>
           <t>EXELON GASOHOL 90</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
+      <c r="K42" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr">
+      <c r="L42" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -2748,53 +2958,58 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>888644</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
           <t>1002685</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>ORGANIZACION FUTURO S.A.C.</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Av. Javier Prado Este 6651, La Molina 15012</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>LA MOLINA</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F43" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G43" t="n">
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
         <v>1000</v>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="I43" t="inlineStr">
         <is>
           <t>40002049</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr">
+      <c r="J43" t="inlineStr">
         <is>
           <t>EXELON NITRO GASOHOL 95</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
+      <c r="K43" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K43" t="inlineStr">
+      <c r="L43" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -2803,53 +3018,58 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>888642</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
           <t>1011179</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>JLF ASOCIADOS S.A.C.</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>Jr Paseo del Bosque 810-890, San Borja 15037</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>SAN BORJA</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F44" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G44" t="n">
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
         <v>1500</v>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="I44" t="inlineStr">
         <is>
           <t>40002039</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
+      <c r="J44" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
-      <c r="J44" t="inlineStr">
+      <c r="K44" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr">
+      <c r="L44" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -2858,53 +3078,58 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>888642</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>1011179</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>JLF ASOCIADOS S.A.C.</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Jr Paseo del Bosque 810-890, San Borja 15037</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>SAN BORJA</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F45" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G45" t="n">
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
         <v>2000</v>
       </c>
-      <c r="H45" t="inlineStr">
+      <c r="I45" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr">
+      <c r="J45" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J45" t="inlineStr">
+      <c r="K45" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr">
+      <c r="L45" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -2913,53 +3138,58 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
+          <t>888642</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>1011179</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>JLF ASOCIADOS S.A.C.</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>Jr Paseo del Bosque 810-890, San Borja 15037</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t>SAN BORJA</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F46" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G46" t="n">
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
         <v>500</v>
       </c>
-      <c r="H46" t="inlineStr">
+      <c r="I46" t="inlineStr">
         <is>
           <t>40002055</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr">
+      <c r="J46" t="inlineStr">
         <is>
           <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
-      <c r="J46" t="inlineStr">
+      <c r="K46" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr">
+      <c r="L46" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -2968,53 +3198,58 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
+          <t>888634</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
           <t>1002685</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="C47" t="inlineStr">
         <is>
           <t>ORGANIZACION FUTURO S.A.C.</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>Av. Javier Prado Este 6651, La Molina 15012</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>LA MOLINA</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F47" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G47" t="n">
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
         <v>500</v>
       </c>
-      <c r="H47" t="inlineStr">
+      <c r="I47" t="inlineStr">
         <is>
           <t>40002023</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
+      <c r="J47" t="inlineStr">
         <is>
           <t>ENDURA DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J47" t="inlineStr">
+      <c r="K47" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K47" t="inlineStr">
+      <c r="L47" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3023,53 +3258,58 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
+          <t>888491</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
           <t>1011063</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="C48" t="inlineStr">
         <is>
           <t>ESTACION DE SERVICIOS NUEVO</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>Av Pachacutec 5295, Villa María del Triunfo 15818</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>VILLA MARIA DEL TRIUNFO</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F48" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G48" t="n">
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
         <v>1000</v>
       </c>
-      <c r="H48" t="inlineStr">
+      <c r="I48" t="inlineStr">
         <is>
           <t>40002039</t>
         </is>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="J48" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
-      <c r="J48" t="inlineStr">
+      <c r="K48" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr">
+      <c r="L48" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3078,53 +3318,58 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>888491</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
           <t>1011063</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="C49" t="inlineStr">
         <is>
           <t>ESTACION DE SERVICIOS NUEVO</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>Av Pachacutec 5295, Villa María del Triunfo 15818</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>VILLA MARIA DEL TRIUNFO</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F49" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G49" t="n">
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
         <v>1000</v>
       </c>
-      <c r="H49" t="inlineStr">
+      <c r="I49" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I49" t="inlineStr">
+      <c r="J49" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J49" t="inlineStr">
+      <c r="K49" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr">
+      <c r="L49" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3133,53 +3378,58 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
+          <t>888490</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
           <t>1011063</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="C50" t="inlineStr">
         <is>
           <t>ESTACION DE SERVICIOS NUEVO</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>Av Pachacutec 5295, Villa María del Triunfo 15818</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>VILLA MARIA DEL TRIUNFO</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F50" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G50" t="n">
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
         <v>1000</v>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="I50" t="inlineStr">
         <is>
           <t>40002019</t>
         </is>
       </c>
-      <c r="I50" t="inlineStr">
+      <c r="J50" t="inlineStr">
         <is>
           <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J50" t="inlineStr">
+      <c r="K50" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr">
+      <c r="L50" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3188,53 +3438,58 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
+          <t>888430</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
           <t>1010564</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="C51" t="inlineStr">
         <is>
           <t>VELDI S.A.</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>Av. Gral. Córdova 1025, Cercado de Lima 15076</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>MIRAFLORES</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F51" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G51" t="n">
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
         <v>500</v>
       </c>
-      <c r="H51" t="inlineStr">
+      <c r="I51" t="inlineStr">
         <is>
           <t>40002019</t>
         </is>
       </c>
-      <c r="I51" t="inlineStr">
+      <c r="J51" t="inlineStr">
         <is>
           <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J51" t="inlineStr">
+      <c r="K51" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr">
+      <c r="L51" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3243,53 +3498,58 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
+          <t>888428</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>1010564</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>VELDI S.A.</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>Av. Gral. Córdova 1025, Cercado de Lima 15076</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>MIRAFLORES</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F52" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G52" t="n">
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
         <v>500</v>
       </c>
-      <c r="H52" t="inlineStr">
+      <c r="I52" t="inlineStr">
         <is>
           <t>40002039</t>
         </is>
       </c>
-      <c r="I52" t="inlineStr">
+      <c r="J52" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
-      <c r="J52" t="inlineStr">
+      <c r="K52" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K52" t="inlineStr">
+      <c r="L52" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3298,53 +3558,58 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
+          <t>888428</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
           <t>1010564</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="C53" t="inlineStr">
         <is>
           <t>VELDI S.A.</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>Av. Gral. Córdova 1025, Cercado de Lima 15076</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>MIRAFLORES</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F53" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G53" t="n">
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
         <v>1500</v>
       </c>
-      <c r="H53" t="inlineStr">
+      <c r="I53" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I53" t="inlineStr">
+      <c r="J53" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J53" t="inlineStr">
+      <c r="K53" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K53" t="inlineStr">
+      <c r="L53" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3353,53 +3618,58 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>888428</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>1010564</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="C54" t="inlineStr">
         <is>
           <t>VELDI S.A.</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>Av. Gral. Córdova 1025, Cercado de Lima 15076</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>MIRAFLORES</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F54" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G54" t="n">
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
         <v>1000</v>
       </c>
-      <c r="H54" t="inlineStr">
+      <c r="I54" t="inlineStr">
         <is>
           <t>40002055</t>
         </is>
       </c>
-      <c r="I54" t="inlineStr">
+      <c r="J54" t="inlineStr">
         <is>
           <t>G-PRIX GASOHOL 97</t>
         </is>
       </c>
-      <c r="J54" t="inlineStr">
+      <c r="K54" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K54" t="inlineStr">
+      <c r="L54" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3408,53 +3678,58 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>888249</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>1010882</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>TRAILER GAS S.A.C.</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>Naranjas 190, Los Olivos 15314</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>SAN MARTÍN DE PORRES</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F55" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G55" t="n">
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
         <v>500</v>
       </c>
-      <c r="H55" t="inlineStr">
+      <c r="I55" t="inlineStr">
         <is>
           <t>40002047</t>
         </is>
       </c>
-      <c r="I55" t="inlineStr">
+      <c r="J55" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 95</t>
         </is>
       </c>
-      <c r="J55" t="inlineStr">
+      <c r="K55" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K55" t="inlineStr">
+      <c r="L55" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3463,53 +3738,58 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>888244</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>1010882</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="C56" t="inlineStr">
         <is>
           <t>TRAILER GAS S.A.C.</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>Naranjas 190, Los Olivos 15314</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>SAN MARTÍN DE PORRES</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F56" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G56" t="n">
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
         <v>500</v>
       </c>
-      <c r="H56" t="inlineStr">
+      <c r="I56" t="inlineStr">
         <is>
           <t>40002039</t>
         </is>
       </c>
-      <c r="I56" t="inlineStr">
+      <c r="J56" t="inlineStr">
         <is>
           <t>PRIMAX GASOHOL 90</t>
         </is>
       </c>
-      <c r="J56" t="inlineStr">
+      <c r="K56" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K56" t="inlineStr">
+      <c r="L56" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3518,53 +3798,58 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>888241</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>1010882</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="C57" t="inlineStr">
         <is>
           <t>TRAILER GAS S.A.C.</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>Naranjas 190, Los Olivos 15314</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>SAN MARTÍN DE PORRES</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F57" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G57" t="n">
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
         <v>2000</v>
       </c>
-      <c r="H57" t="inlineStr">
+      <c r="I57" t="inlineStr">
         <is>
           <t>40002019</t>
         </is>
       </c>
-      <c r="I57" t="inlineStr">
+      <c r="J57" t="inlineStr">
         <is>
           <t>MAX-D DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J57" t="inlineStr">
+      <c r="K57" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr">
+      <c r="L57" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>
@@ -3573,53 +3858,58 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>887576</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>1012165</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
+      <c r="C58" t="inlineStr">
         <is>
           <t>TURISMO CIVA S.A.C.</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>Sancho de Rivera 1184, Cercado de Lima 15001</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>CERCADO DE LIMA</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>LIMA</t>
-        </is>
-      </c>
       <c r="F58" t="inlineStr">
         <is>
           <t>LIMA</t>
         </is>
       </c>
-      <c r="G58" t="n">
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>LIMA</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
         <v>6500</v>
       </c>
-      <c r="H58" t="inlineStr">
+      <c r="I58" t="inlineStr">
         <is>
           <t>40002021</t>
         </is>
       </c>
-      <c r="I58" t="inlineStr">
+      <c r="J58" t="inlineStr">
         <is>
           <t>MAX-P DIESEL B5 S50 UV</t>
         </is>
       </c>
-      <c r="J58" t="inlineStr">
+      <c r="K58" t="inlineStr">
         <is>
           <t>P614</t>
         </is>
       </c>
-      <c r="K58" t="inlineStr">
+      <c r="L58" t="inlineStr">
         <is>
           <t>TERMINAL PBF CALLAO</t>
         </is>

</xml_diff>